<commit_message>
ATT: arrumado erros nas contas basicas
</commit_message>
<xml_diff>
--- a/teste_de casos_juros_compostos.xlsx
+++ b/teste_de casos_juros_compostos.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20343"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\facar\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\CALCULAR_JUROS_COMPOSTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F05AD3-9A90-4DFC-8405-FBDC4E6B53C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3295423-127A-4954-944D-C683927188A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{61A05F25-93FB-48C3-817C-B9B93562EB45}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Caso de Teste" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>Arquivos</t>
   </si>
@@ -71,112 +60,103 @@
     <t>(200 = juros, 1200 = montante)</t>
   </si>
   <si>
+    <t>Enviando o valor do juros como decimal</t>
+  </si>
+  <si>
+    <t>1000, 15.5, 1</t>
+  </si>
+  <si>
+    <t>(155, 1155)</t>
+  </si>
+  <si>
+    <t>Não enviando o valor da capital</t>
+  </si>
+  <si>
+    <t>20, 2</t>
+  </si>
+  <si>
+    <t>ValueError("Não é possível fazer a conta sem o valor da capital")</t>
+  </si>
+  <si>
+    <t>Não enviando o valor da taxa de juros</t>
+  </si>
+  <si>
+    <t>1000, 2</t>
+  </si>
+  <si>
+    <t>ValueError("Não é possível fazer a conta sem o valor da taxa de juros")</t>
+  </si>
+  <si>
+    <t>Não enviando o valor do tempo</t>
+  </si>
+  <si>
+    <t>1000, 30</t>
+  </si>
+  <si>
+    <t>ValueError("Não é possível fazer a conta sem o valor do tempo")</t>
+  </si>
+  <si>
     <t>Testando envio de tupla vazia</t>
   </si>
   <si>
     <t>()</t>
   </si>
   <si>
-    <t>ValueError("Não é permitido uma lista vazia")</t>
-  </si>
-  <si>
-    <t>Enviando com valores insuficientes</t>
-  </si>
-  <si>
-    <t>1000, 20</t>
-  </si>
-  <si>
-    <t>ValueError("Não é possível fazer a conta com números insuficientes")</t>
-  </si>
-  <si>
-    <t>1000, 15.5, 1</t>
-  </si>
-  <si>
-    <t>(155, 1155)</t>
-  </si>
-  <si>
-    <t>Enviando o valor do juros como decimal</t>
-  </si>
-  <si>
     <t>Enviando uma string como valor da capital</t>
   </si>
   <si>
+    <t>"oiii", 25, 2</t>
+  </si>
+  <si>
     <t>ValueError("O valor do capital precisa ser int ou float")</t>
   </si>
   <si>
     <t>Enviando uma string como valor dos juros</t>
   </si>
   <si>
+    <t xml:space="preserve"> 2600, "oiii", 3</t>
+  </si>
+  <si>
     <t>ValueError("O valor dos juros precisa ser int ou float")</t>
   </si>
   <si>
+    <t>Enviando uma string como valor do tempo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2700, 4,"oiii"</t>
+  </si>
+  <si>
     <t>ValueError("O valor do tempo precisa ser int ou float")</t>
   </si>
   <si>
-    <t>Enviando uma string como valor do tempo</t>
-  </si>
-  <si>
     <t>Enviando um valor da capital negativo</t>
   </si>
   <si>
+    <t>-2000, 30, 3</t>
+  </si>
+  <si>
+    <t>ValueError("Não é permitido o valor da capital &lt; que 0")</t>
+  </si>
+  <si>
     <t>Enviando um valor dos juros negativo</t>
   </si>
   <si>
+    <t>2000, -30, 3</t>
+  </si>
+  <si>
+    <t>ValueError("Não é permitido o valor dos juros &lt; que 0")</t>
+  </si>
+  <si>
     <t>Enviando um valor do tempo negativo</t>
   </si>
   <si>
-    <t>ValueError("Não é permitido o valor da capital &lt; que 0")</t>
-  </si>
-  <si>
-    <t>ValueError("Não é permitido o valor dos juros &lt; que 0")</t>
+    <t>2000, 30, -3</t>
   </si>
   <si>
     <t>ValueError("Não é permitido o valor do tempo &lt; que 0")</t>
   </si>
   <si>
-    <t>Enviando o numero 0 como capital</t>
-  </si>
-  <si>
-    <t>0, 20, 3</t>
-  </si>
-  <si>
-    <t>Enviando o numero 0 como juros</t>
-  </si>
-  <si>
-    <t>Enviando o numero 0 como tempo</t>
-  </si>
-  <si>
-    <t>3000, 20, 0</t>
-  </si>
-  <si>
-    <t>2000, 0, 3</t>
-  </si>
-  <si>
-    <t>"oiii", 25, 2</t>
-  </si>
-  <si>
-    <t>2000, -30, 3</t>
-  </si>
-  <si>
-    <t>2000, 30, -3</t>
-  </si>
-  <si>
-    <t>-2000, 30, 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2600, "oiii", 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2700, 4,"oiii"</t>
-  </si>
-  <si>
-    <t>ValueError("Não é permitido o valor do tempo = 0")</t>
-  </si>
-  <si>
-    <t>ValueError("Não é permitido o valor da capital =  0")</t>
-  </si>
-  <si>
-    <t>ValueError("Não é permitido o valor dos juros = 0")</t>
+    <t>ValueError("Não é permitido uma tupla vazia")</t>
   </si>
 </sst>
 </file>
@@ -353,9 +333,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -393,7 +373,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -499,7 +479,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -641,7 +621,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -649,17 +629,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A115FB1-5C3E-4012-B6E8-6823848665B0}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="57.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -708,13 +688,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -742,13 +722,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -762,10 +742,10 @@
         <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -776,13 +756,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -796,10 +776,10 @@
         <v>25</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -810,13 +790,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>41</v>
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -827,13 +807,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -844,13 +824,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -861,13 +841,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -878,30 +858,13 @@
         <v>6</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>